<commit_message>
slides de custo e gamma Signed-off-by: leonardomedeiros <leonardomelomedeiros@gmail.com>
</commit_message>
<xml_diff>
--- a/gqm/gqm-graficos.xlsx
+++ b/gqm/gqm-graficos.xlsx
@@ -5,19 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="311" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="311" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Gráficos" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Gráfico Diversao" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Plan3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Grafico Frequencia" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Gráfico Faixa Etaria" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="66">
   <si>
     <t>Indicação de data e hora</t>
   </si>
@@ -206,6 +208,15 @@
   </si>
   <si>
     <t>Escala 5</t>
+  </si>
+  <si>
+    <t>3 vezes ao dia</t>
+  </si>
+  <si>
+    <t>Qual a sua opinião sobre a faixa etária do jogo ?</t>
+  </si>
+  <si>
+    <t>Adultos</t>
   </si>
 </sst>
 </file>
@@ -217,7 +228,7 @@
     <numFmt numFmtId="165" formatCode="D/M/YYYY\ HH:MM"/>
     <numFmt numFmtId="166" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -275,8 +286,17 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Linux Libertine Display O"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -395,7 +415,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -441,6 +461,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,7 +540,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -554,7 +578,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -587,7 +611,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Gráficos!$C$2</c:f>
+              <c:f>'Gráfico Diversao'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -702,7 +726,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Gráficos!$B$3:$B$6</c:f>
+              <c:f>'Gráfico Diversao'!$B$3:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -722,7 +746,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Gráficos!$C$3:$C$6</c:f>
+              <c:f>'Gráfico Diversao'!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -753,16 +777,431 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="2400">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Se você tivesse adquirido esse jogo, 
+com que frequencia você o utilizaria durante a semana?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Grafico Frequencia'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Grafico Frequencia'!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1 vez</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 vezes ao dia</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Todos os dias</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Grafico Frequencia'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
         </a:ln>
       </c:spPr>
-    </c:legend>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="2400">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Qual a sua opinião sobre a faixa etária do jogo ?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico Faixa Etaria'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:separator>
+</c:separator>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Gráfico Faixa Etaria'!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Livre</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Adultos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Crianças</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico Faixa Etaria'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:spPr>
@@ -782,14 +1221,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>739080</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2167560</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -817,14 +1256,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>421560</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -832,7 +1271,77 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5524920" y="841320"/>
+        <a:off x="5524920" y="949320"/>
+        <a:ext cx="9527400" cy="6568200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>421560</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>141480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5524920" y="949320"/>
+        <a:ext cx="9527400" cy="6568200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>73080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>421560</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5524920" y="949320"/>
         <a:ext cx="9527400" cy="6568200"/>
       </xdr:xfrm>
       <a:graphic>
@@ -854,10 +1363,10 @@
   </sheetPr>
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1255,7 +1764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
@@ -1749,7 +2258,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>56</v>
       </c>
@@ -1879,8 +2388,8 @@
   </sheetPr>
   <dimension ref="B2:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S28" activeCellId="0" sqref="S28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1956,7 +2465,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1965,4 +2477,126 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:C65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S11" activeCellId="0" sqref="S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.53441295546559"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:C65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S17" activeCellId="0" sqref="S17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.53441295546559"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>